<commit_message>
Smaller masks (fROI + anatomical) + better output
</commit_message>
<xml_diff>
--- a/HCP_group_effect_sizes/EffectSize/es.xlsx
+++ b/HCP_group_effect_sizes/EffectSize/es.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="1140" windowWidth="24220" windowHeight="12580" tabRatio="500"/>
+    <workbookView xWindow="18600" yWindow="180" windowWidth="30920" windowHeight="19400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="es.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>Paradigm</t>
   </si>
@@ -78,9 +78,6 @@
     <t>contrast</t>
   </si>
   <si>
-    <t>mask (from Harvard-oxford)</t>
-  </si>
-  <si>
     <t>mask size</t>
   </si>
   <si>
@@ -91,13 +88,37 @@
   </si>
   <si>
     <t>Percent BOLD change</t>
+  </si>
+  <si>
+    <t>MOTOR</t>
+  </si>
+  <si>
+    <t>Precentral Gyrus</t>
+  </si>
+  <si>
+    <t>Middle frontal gyrus</t>
+  </si>
+  <si>
+    <t>EMOTION</t>
+  </si>
+  <si>
+    <t>GAMBLING</t>
+  </si>
+  <si>
+    <t>mask: P&gt;0</t>
+  </si>
+  <si>
+    <t>and neurosynth</t>
+  </si>
+  <si>
+    <t>mask: P&gt;0.25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -118,8 +139,24 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,6 +166,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -142,14 +185,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -163,8 +211,28 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -494,330 +562,673 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="3"/>
-    <col min="2" max="2" width="15.1640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="29.1640625" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="15.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G2" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="H2" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4">
+        <v>29115</v>
+      </c>
+      <c r="E3" s="5">
+        <v>-2.4256925843656001E-2</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.18762100000000001</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.41498791873454999</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>2.3860000000000001</v>
+      </c>
+      <c r="J3" s="5">
+        <v>8.2070000000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4">
+        <v>5970</v>
+      </c>
+      <c r="E4" s="5">
+        <v>4.60015296936035E-2</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.207841</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.36587106585502599</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0.55710000000000004</v>
+      </c>
+      <c r="I4" s="5">
+        <v>4.7160000000000002</v>
+      </c>
+      <c r="J4" s="5">
+        <v>14.79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3168</v>
+      </c>
+      <c r="E5" s="5">
+        <v>-2.0346078649163199E-2</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.12395200000000001</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0.26593430340289997</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0.1081</v>
+      </c>
+      <c r="I5" s="5">
+        <v>2.508</v>
+      </c>
+      <c r="J5" s="5">
+        <v>4.33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3207</v>
+      </c>
+      <c r="E6" s="5">
+        <v>-4.3845877796411498E-2</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.10093100000000001</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.25102442502975397</v>
+      </c>
+      <c r="H6" s="5">
+        <v>-0.39629999999999999</v>
+      </c>
+      <c r="I6" s="5">
+        <v>1.889</v>
+      </c>
+      <c r="J6" s="5">
+        <v>3.597</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="4">
+        <v>18250</v>
+      </c>
+      <c r="E7" s="5">
+        <v>-1.1770450416952301E-2</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.17175599999999999</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.35277226567268299</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0.14280000000000001</v>
+      </c>
+      <c r="I7" s="5">
+        <v>1.0389999999999999</v>
+      </c>
+      <c r="J7" s="5">
+        <v>2.8130000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1864</v>
+      </c>
+      <c r="E8" s="5">
+        <v>5.1099266856908701E-2</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.20005700000000001</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0.39616224169731101</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1.5095000000000001</v>
+      </c>
+      <c r="J8" s="5">
+        <v>3.83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2083</v>
+      </c>
+      <c r="E9" s="5">
+        <v>6.0025349259376498E-2</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.217117</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.42589215934276498</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1.5920000000000001</v>
+      </c>
+      <c r="J9" s="5">
+        <v>4.0385</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="4">
+        <v>820</v>
+      </c>
+      <c r="E10" s="5">
+        <v>3.2833870872855102E-2</v>
+      </c>
+      <c r="F10" s="5">
+        <v>8.9571399999999995E-2</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.14404181540012301</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0.38965</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="J10" s="5">
+        <v>1.2669999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="C11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="4">
+        <v>762</v>
+      </c>
+      <c r="E11" s="5">
+        <v>2.8685585409402799E-2</v>
+      </c>
+      <c r="F11" s="5">
+        <v>8.8916200000000001E-2</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0.14705739170312801</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0.4294</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="J11" s="5">
+        <v>1.5329999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="H2" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="4">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="5">
-        <v>29115</v>
-      </c>
-      <c r="E3" s="6">
-        <v>-2.4256925843656001E-2</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0.18762100000000001</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0.41498791873454999</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0</v>
-      </c>
-      <c r="I3" s="6">
-        <v>2.3860000000000001</v>
-      </c>
-      <c r="J3" s="6">
-        <v>8.2070000000000007</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="C4" s="3" t="s">
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="4">
+        <v>12894</v>
+      </c>
+      <c r="E16" s="5">
+        <v>6.9293133914470603E-2</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.25318099999999999</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0.45556858181953402</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0.50460000000000005</v>
+      </c>
+      <c r="I16" s="5">
+        <v>2.7069999999999999</v>
+      </c>
+      <c r="J16" s="5">
+        <v>8.5820000000000007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5">
-        <v>5970</v>
-      </c>
-      <c r="E4" s="6">
-        <v>4.60015296936035E-2</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0.207841</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0.36587106585502599</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0.55710000000000004</v>
-      </c>
-      <c r="I4" s="6">
-        <v>4.7160000000000002</v>
-      </c>
-      <c r="J4" s="6">
-        <v>14.79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="C5" s="3" t="s">
+      <c r="D17" s="4">
+        <v>3418</v>
+      </c>
+      <c r="E17" s="5">
+        <v>7.3651073127984995E-2</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.23594499999999999</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0.367990246415138</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0.91049999999999998</v>
+      </c>
+      <c r="I17" s="5">
+        <v>4.0330000000000004</v>
+      </c>
+      <c r="J17" s="5">
+        <v>12.51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="5">
-        <v>3168</v>
-      </c>
-      <c r="E5" s="6">
-        <v>-2.0346078649163199E-2</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0.12395200000000001</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0.26593430340289997</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0.1081</v>
-      </c>
-      <c r="I5" s="6">
-        <v>2.508</v>
-      </c>
-      <c r="J5" s="6">
-        <v>4.33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="C6" s="3" t="s">
+      <c r="D18" s="4">
+        <v>1351</v>
+      </c>
+      <c r="E18" s="5">
+        <v>3.94500643014907E-2</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.17968700000000001</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0.30131018161773598</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0.68910000000000005</v>
+      </c>
+      <c r="I18" s="5">
+        <v>2.5169999999999999</v>
+      </c>
+      <c r="J18" s="5">
+        <v>4.3380000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="5">
-        <v>3207</v>
-      </c>
-      <c r="E6" s="6">
-        <v>-4.3845877796411498E-2</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0.10093100000000001</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0.25102442502975397</v>
-      </c>
-      <c r="H6" s="6">
-        <v>-0.39629999999999999</v>
-      </c>
-      <c r="I6" s="6">
-        <v>1.889</v>
-      </c>
-      <c r="J6" s="6">
-        <v>3.597</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="3" t="s">
+      <c r="D19" s="4">
+        <v>1280</v>
+      </c>
+      <c r="E19" s="5">
+        <v>1.4702468411997001E-3</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.134351</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0.27122366130351999</v>
+      </c>
+      <c r="H19" s="5">
+        <v>2.6409999999999999E-2</v>
+      </c>
+      <c r="I19" s="5">
+        <v>1.8129999999999999</v>
+      </c>
+      <c r="J19" s="5">
+        <v>3.661</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="5">
-        <v>18250</v>
-      </c>
-      <c r="E7" s="6">
-        <v>-1.1770450416952301E-2</v>
-      </c>
-      <c r="F7" s="6">
-        <v>0.17175599999999999</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0.35277226567268299</v>
-      </c>
-      <c r="H7" s="6">
-        <v>0.14280000000000001</v>
-      </c>
-      <c r="I7" s="6">
-        <v>1.0389999999999999</v>
-      </c>
-      <c r="J7" s="6">
-        <v>2.8130000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="4">
+        <v>204</v>
+      </c>
+      <c r="E20" s="5">
+        <v>3.6184743419289497E-2</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0.16075</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0.483536803722381</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0.19755</v>
+      </c>
+      <c r="I20" s="5">
+        <v>1.0015000000000001</v>
+      </c>
+      <c r="J20" s="5">
+        <v>2.3260000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C21" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="5">
-        <v>1864</v>
-      </c>
-      <c r="E8" s="6">
-        <v>5.1099266856908701E-2</v>
-      </c>
-      <c r="F8" s="6">
-        <v>0.20005700000000001</v>
-      </c>
-      <c r="G8" s="6">
-        <v>0.39616224169731101</v>
-      </c>
-      <c r="H8" s="6">
-        <v>0.72099999999999997</v>
-      </c>
-      <c r="I8" s="6">
-        <v>1.5095000000000001</v>
-      </c>
-      <c r="J8" s="6">
-        <v>3.83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="C9" s="3" t="s">
+      <c r="D21" s="4">
+        <v>1003</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.15559004247188499</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0.30232199999999998</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0.46736234426498402</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="I21" s="5">
+        <v>1.3995</v>
+      </c>
+      <c r="J21" s="5">
+        <v>3.7124999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="5">
-        <v>2083</v>
-      </c>
-      <c r="E9" s="6">
-        <v>6.0025349259376498E-2</v>
-      </c>
-      <c r="F9" s="6">
-        <v>0.217117</v>
-      </c>
-      <c r="G9" s="6">
-        <v>0.42589215934276498</v>
-      </c>
-      <c r="H9" s="6">
-        <v>0.71899999999999997</v>
-      </c>
-      <c r="I9" s="6">
-        <v>1.5920000000000001</v>
-      </c>
-      <c r="J9" s="6">
-        <v>4.0385</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="D22" s="4">
+        <v>1082</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0.13540638834238</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0.292495</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0.46550558209419202</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0.94350000000000001</v>
+      </c>
+      <c r="I22" s="5">
+        <v>1.7635000000000001</v>
+      </c>
+      <c r="J22" s="5">
+        <v>4.4775</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C23" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="5">
-        <v>820</v>
-      </c>
-      <c r="E10" s="6">
-        <v>3.2833870872855102E-2</v>
-      </c>
-      <c r="F10" s="6">
-        <v>8.9571399999999995E-2</v>
-      </c>
-      <c r="G10" s="6">
-        <v>0.14404181540012301</v>
-      </c>
-      <c r="H10" s="6">
-        <v>0.38965</v>
-      </c>
-      <c r="I10" s="6">
-        <v>0.78800000000000003</v>
-      </c>
-      <c r="J10" s="6">
-        <v>1.2669999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="C11" s="3" t="s">
+      <c r="D23" s="4">
+        <v>346</v>
+      </c>
+      <c r="E23" s="5">
+        <v>4.6026155352592399E-2</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0.10677200000000001</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0.163993120193481</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0.42745</v>
+      </c>
+      <c r="I23" s="5">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="J23" s="5">
+        <v>1.6185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="5">
-        <v>762</v>
-      </c>
-      <c r="E11" s="6">
-        <v>2.8685585409402799E-2</v>
-      </c>
-      <c r="F11" s="6">
-        <v>8.8916200000000001E-2</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0.14705739170312801</v>
-      </c>
-      <c r="H11" s="6">
-        <v>0.4294</v>
-      </c>
-      <c r="I11" s="6">
-        <v>0.96499999999999997</v>
-      </c>
-      <c r="J11" s="6">
-        <v>1.5329999999999999</v>
+      <c r="D24" s="4">
+        <v>346</v>
+      </c>
+      <c r="E24" s="5">
+        <v>4.6026155352592399E-2</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0.10677200000000001</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0.163993120193481</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0.42745</v>
+      </c>
+      <c r="I24" s="5">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="J24" s="5">
+        <v>1.6185</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:J14"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>